<commit_message>
All the completed files
</commit_message>
<xml_diff>
--- a/ComparisonResults.xlsx
+++ b/ComparisonResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zunayed\Desktop\Third year\Third Year Project\IntentRecognition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA12A0E2-56C6-4A7D-AD53-AAF778830128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DCD41A-9912-44A2-B659-E68CB5AA884F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{A46324FF-687F-4F3B-81DE-90CC1D4E9A5E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="12">
   <si>
     <t>Goals</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>Observation</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Googlemaps</t>
   </si>
 </sst>
 </file>
@@ -359,16 +365,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.96</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.96</c:v>
+                  <c:v>0.84</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.88</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.76</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -637,6 +643,501 @@
           <c:y val="0.81572663511178312"/>
           <c:w val="0.11527358315392221"/>
           <c:h val="7.7187490320679938E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Google Maps (Baseline with</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> landmarks)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AR$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TPR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$AQ$34:$AQ$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AR$34:$AR$38</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EE8A-48BA-848A-A278CA3211EB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1641839232"/>
+        <c:axId val="1641849792"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1641839232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Observations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.44176968503937009"/>
+              <c:y val="0.77277704870224551"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1641849792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1641849792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>TPR</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1641839232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.45108880139982505"/>
+          <c:y val="0.86631889763779524"/>
+          <c:w val="0.12560017497812773"/>
+          <c:h val="7.8125546806649182E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1229,7 +1730,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>LLM (observation)</a:t>
+              <a:t>LLM (as observation agent)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3728,10 +4229,10 @@
                   <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.85</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.85</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.7</c:v>
@@ -4072,7 +4573,532 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Google</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Maps (Baseline with landmarks)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AR$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TPR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$AQ$6:$AQ$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AR$6:$AR$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-264F-4031-AE61-8CB91EE0846A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1507540592"/>
+        <c:axId val="1507533392"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1507540592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Goals</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1507533392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1507533392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>TPR</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1507540592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.4371999125109361"/>
+          <c:y val="0.80613371245261012"/>
+          <c:w val="0.12560017497812773"/>
+          <c:h val="7.8125546806649182E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4392,6 +5418,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -4908,7 +5974,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5424,7 +6490,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5940,7 +7006,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6456,7 +7522,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6972,7 +8038,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7488,7 +8554,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8004,7 +9070,1039 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8810,6 +10908,78 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E53DFC1-1C34-9376-ED42-65E68C11991A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>223837</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>528637</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBC0B7FE-CFE5-6752-E916-72BFEDA67F12}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9130,10 +11300,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F97FD78-AEA6-4922-BF37-B8F6C6EA7594}">
-  <dimension ref="B4:AH39"/>
+  <dimension ref="B4:AT39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O28" workbookViewId="0">
-      <selection activeCell="AM53" sqref="AM53"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AK7" sqref="AK7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9144,7 +11314,7 @@
     <col min="31" max="31" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
@@ -9167,8 +11337,15 @@
         <v>6</v>
       </c>
       <c r="AH4" s="6"/>
+      <c r="AR4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AS4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AT4" s="6"/>
     </row>
-    <row r="5" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -9217,19 +11394,31 @@
       <c r="AH5" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="AQ5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT5" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="6" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2</v>
       </c>
       <c r="C6" s="4">
-        <v>0.96</v>
+        <v>0.94</v>
       </c>
       <c r="D6" s="4">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="E6" s="7">
-        <v>0.96</v>
+        <v>0.94</v>
       </c>
       <c r="N6" s="1">
         <v>2</v>
@@ -9267,19 +11456,31 @@
       <c r="AH6" s="4">
         <v>0.8</v>
       </c>
+      <c r="AQ6" s="1">
+        <v>2</v>
+      </c>
+      <c r="AR6" s="4">
+        <v>0.92</v>
+      </c>
+      <c r="AS6" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="AT6" s="4">
+        <v>0.92</v>
+      </c>
     </row>
-    <row r="7" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>5</v>
       </c>
       <c r="C7" s="4">
-        <v>0.96</v>
+        <v>0.84</v>
       </c>
       <c r="D7" s="4">
-        <v>0.04</v>
+        <v>0.16</v>
       </c>
       <c r="E7" s="7">
-        <v>0.96</v>
+        <v>0.9</v>
       </c>
       <c r="N7" s="1">
         <v>5</v>
@@ -9317,16 +11518,28 @@
       <c r="AH7" s="4">
         <v>0.2</v>
       </c>
+      <c r="AQ7" s="1">
+        <v>5</v>
+      </c>
+      <c r="AR7" s="4">
+        <v>0.84</v>
+      </c>
+      <c r="AS7" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="AT7" s="4">
+        <v>0.84</v>
+      </c>
     </row>
-    <row r="8" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>10</v>
       </c>
       <c r="C8" s="4">
-        <v>0.88</v>
+        <v>0.8</v>
       </c>
       <c r="D8" s="4">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="E8" s="7">
         <v>0.88</v>
@@ -9367,16 +11580,28 @@
       <c r="AH8" s="4">
         <v>0</v>
       </c>
+      <c r="AQ8" s="1">
+        <v>10</v>
+      </c>
+      <c r="AR8" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="AS8" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AT8" s="4">
+        <v>0.8</v>
+      </c>
     </row>
-    <row r="9" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>15</v>
       </c>
       <c r="C9" s="4">
-        <v>0.76</v>
+        <v>0.7</v>
       </c>
       <c r="D9" s="4">
-        <v>0.24</v>
+        <v>0.3</v>
       </c>
       <c r="E9" s="7">
         <v>0.76</v>
@@ -9417,8 +11642,29 @@
       <c r="AH9" s="4">
         <v>0.2</v>
       </c>
+      <c r="AQ9" s="1">
+        <v>15</v>
+      </c>
+      <c r="AR9" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="AS9" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AT9" s="4">
+        <v>0.8</v>
+      </c>
     </row>
-    <row r="33" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="44:46" x14ac:dyDescent="0.25">
+      <c r="AR32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AS32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AT32" s="6"/>
+    </row>
+    <row r="33" spans="2:46" x14ac:dyDescent="0.25">
       <c r="C33" s="5" t="s">
         <v>4</v>
       </c>
@@ -9445,8 +11691,20 @@
         <v>6</v>
       </c>
       <c r="AH33" s="6"/>
+      <c r="AQ33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AR33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT33" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="34" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>7</v>
       </c>
@@ -9495,8 +11753,22 @@
       <c r="AH34" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="AQ34" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR34" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="AS34" s="4">
+        <f>1-AR34</f>
+        <v>0.4</v>
+      </c>
+      <c r="AT34" s="4">
+        <f>AR34</f>
+        <v>0.6</v>
+      </c>
     </row>
-    <row r="35" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
         <v>1</v>
       </c>
@@ -9504,6 +11776,7 @@
         <v>0.6</v>
       </c>
       <c r="D35" s="4">
+        <f>1-C35</f>
         <v>0.4</v>
       </c>
       <c r="E35" s="4">
@@ -9545,16 +11818,31 @@
       <c r="AH35" s="4">
         <v>0.43</v>
       </c>
+      <c r="AQ35" s="1">
+        <v>3</v>
+      </c>
+      <c r="AR35" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="AS35" s="4">
+        <f t="shared" ref="AS35:AS38" si="0">1-AR35</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AT35" s="4">
+        <f t="shared" ref="AT35:AT38" si="1">AR35</f>
+        <v>0.85</v>
+      </c>
     </row>
-    <row r="36" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
         <v>3</v>
       </c>
       <c r="C36" s="4">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
       <c r="D36" s="4">
-        <v>0.15</v>
+        <f t="shared" ref="D36:D39" si="2">1-C36</f>
+        <v>0.19999999999999996</v>
       </c>
       <c r="E36" s="4">
         <v>0.85</v>
@@ -9595,16 +11883,31 @@
       <c r="AH36" s="4">
         <v>0.43</v>
       </c>
+      <c r="AQ36" s="1">
+        <v>5</v>
+      </c>
+      <c r="AR36" s="4">
+        <v>1</v>
+      </c>
+      <c r="AS36" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT36" s="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <v>5</v>
       </c>
       <c r="C37" s="4">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
       <c r="D37" s="4">
-        <v>0.15</v>
+        <f t="shared" si="2"/>
+        <v>0.19999999999999996</v>
       </c>
       <c r="E37" s="4">
         <v>0.85</v>
@@ -9645,8 +11948,22 @@
       <c r="AH37" s="4">
         <v>0.14000000000000001</v>
       </c>
+      <c r="AQ37" s="1">
+        <v>10</v>
+      </c>
+      <c r="AR37" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="AS37" s="4">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="AT37" s="4">
+        <f t="shared" si="1"/>
+        <v>0.9</v>
+      </c>
     </row>
-    <row r="38" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
         <v>10</v>
       </c>
@@ -9654,7 +11971,8 @@
         <v>0.7</v>
       </c>
       <c r="D38" s="4">
-        <v>0.3</v>
+        <f t="shared" si="2"/>
+        <v>0.30000000000000004</v>
       </c>
       <c r="E38" s="4">
         <v>0.7</v>
@@ -9695,8 +12013,22 @@
       <c r="AH38" s="4">
         <v>0.28999999999999998</v>
       </c>
+      <c r="AQ38" s="1">
+        <v>15</v>
+      </c>
+      <c r="AR38" s="4">
+        <v>1</v>
+      </c>
+      <c r="AS38" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AT38" s="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="39" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <v>15</v>
       </c>
@@ -9704,7 +12036,8 @@
         <v>0.85</v>
       </c>
       <c r="D39" s="4">
-        <v>0.15</v>
+        <f t="shared" si="2"/>
+        <v>0.15000000000000002</v>
       </c>
       <c r="E39" s="4">
         <v>0.85</v>

</xml_diff>